<commit_message>
Atualização automática via Streamlit (13/11/2025 17:43)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -2,27 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="PRINCIPAL" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -33,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,15 +45,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,78 +425,93 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A2:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="38.1796875" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="21.90625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="18.36328125" bestFit="1" customWidth="1" min="11" max="11"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>UF</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>FRU</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>SUB1</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SUB2</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>SUB3</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>DESCRICAO</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>MAQUINAS</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>CLIENTES</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>DATA FIM DE CONTRATO</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>SLA</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>DATA VER. SEMANAL</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CONTRATO</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>CLIENTE</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_FIM</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_VERIFICACAO</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
         </is>
       </c>
     </row>
@@ -528,6 +556,64 @@
         </is>
       </c>
       <c r="L2" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00x0001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>12h</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>teste - (teste 01/11/25_12h) - PA</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>DENTRO</t>
         </is>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 17:56)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,6 +619,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00p0003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>fonte</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>xuxa</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>xoxo - (xxxoxox 02/11/25_12h) - AM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>12h</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>02/11/25</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 18:54)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -1,106 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Robo_Pecas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E554AF-98D2-48C8-B55F-D0D99E146DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PRINCIPAL" sheetId="1" r:id="rId1"/>
+    <sheet name="PRINCIPAL" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>FRU</t>
-  </si>
-  <si>
-    <t>SUB1</t>
-  </si>
-  <si>
-    <t>SUB2</t>
-  </si>
-  <si>
-    <t>SUB3</t>
-  </si>
-  <si>
-    <t>DESCRICAO</t>
-  </si>
-  <si>
-    <t>MAQUINAS</t>
-  </si>
-  <si>
-    <t>CLIENTES</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>00X0090</t>
-  </si>
-  <si>
-    <t>TESTE</t>
-  </si>
-  <si>
-    <t>TESTE - (TESTE 28/11/25_) - TO</t>
-  </si>
-  <si>
-    <t>28/11/25</t>
-  </si>
-  <si>
-    <t>10/11/25</t>
-  </si>
-  <si>
-    <t>DENTRO</t>
-  </si>
-  <si>
-    <t>DATA_VERIFICACAO</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>DATA_FIM</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,26 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -415,82 +420,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>UF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FRU</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SUB1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SUB2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SUB3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DESCRICAO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MAQUINAS</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CLIENTES</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_FIM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SLA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_VERIFICACAO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>CLIENTE</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>00X0090</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>TESTE - (TESTE 28/11/25_) - TO</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>28/11/25</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10/11/25</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00p0001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fonte</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2530</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>12h</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>xuxa - (7809876 01/11/25_12h) - AM</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 18:57)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -1,106 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Robo_Pecas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B32472-141B-42D6-A0E4-180FCE4A63CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PRINCIPAL" sheetId="1" r:id="rId1"/>
+    <sheet name="PRINCIPAL" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>FRU</t>
-  </si>
-  <si>
-    <t>SUB1</t>
-  </si>
-  <si>
-    <t>SUB2</t>
-  </si>
-  <si>
-    <t>SUB3</t>
-  </si>
-  <si>
-    <t>DESCRICAO</t>
-  </si>
-  <si>
-    <t>MAQUINAS</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>TO</t>
-  </si>
-  <si>
-    <t>00X0090</t>
-  </si>
-  <si>
-    <t>TESTE</t>
-  </si>
-  <si>
-    <t>TESTE - (TESTE 28/11/25_) - TO</t>
-  </si>
-  <si>
-    <t>28/11/25</t>
-  </si>
-  <si>
-    <t>10/11/25</t>
-  </si>
-  <si>
-    <t>DENTRO</t>
-  </si>
-  <si>
-    <t>DATA_VERIFICACAO</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>DATA_FIM</t>
-  </si>
-  <si>
-    <t>CLIENTE</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,26 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -415,82 +420,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>UF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FRU</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SUB1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SUB2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SUB3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DESCRICAO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MAQUINAS</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CLIENTE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_FIM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SLA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_VERIFICACAO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>00X0090</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>TESTE - (TESTE 28/11/25_) - TO</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>28/11/25</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10/11/25</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00p0001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>x - (x 01/11/25_12h) - AM</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>12h</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 19:00)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -549,7 +549,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>00p0001</t>
+          <t>00p0012</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -557,27 +557,27 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>k</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>k</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>x - (x 01/11/25_12h) - AM</t>
+          <t>k - (k 01/10/25_24h) - AM</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>01/11/25</t>
+          <t>01/10/25</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>12h</t>
+          <t>24h</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 19:09)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,6 +591,56 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00x0098</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>p - (p 01/08/25_24h) - AM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>01/08/25</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>24h</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 19:40)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -1,121 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Robo_Pecas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A12C39-683C-452D-A5E3-E7CD85CF7858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PRINCIPAL" sheetId="1" r:id="rId1"/>
+    <sheet name="PRINCIPAL" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>FRU</t>
-  </si>
-  <si>
-    <t>SUB1</t>
-  </si>
-  <si>
-    <t>SUB2</t>
-  </si>
-  <si>
-    <t>SUB3</t>
-  </si>
-  <si>
-    <t>DESCRICAO</t>
-  </si>
-  <si>
-    <t>MAQUINAS</t>
-  </si>
-  <si>
-    <t>SLA</t>
-  </si>
-  <si>
-    <t>DENTRO</t>
-  </si>
-  <si>
-    <t>DATA_VERIFICACAO</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>DATA_FIM</t>
-  </si>
-  <si>
-    <t>CLIENTE</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>00p0012</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>k - (k 01/10/25_24h) - AM</t>
-  </si>
-  <si>
-    <t>01/10/25</t>
-  </si>
-  <si>
-    <t>24h</t>
-  </si>
-  <si>
-    <t>13/11/25</t>
-  </si>
-  <si>
-    <t>00x0098</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>p - (p 01/08/25_24h) - AM</t>
-  </si>
-  <si>
-    <t>01/08/25</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,26 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -430,114 +420,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>UF</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>FRU</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SUB1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>SUB2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SUB3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DESCRICAO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MAQUINAS</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CLIENTE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_FIM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>SLA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_VERIFICACAO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>00p0012</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>k - (k 01/10/25_24h) - AM</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>01/10/25</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>24h</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00x0098</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>p</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>p - (p 01/08/25_24h) - AM</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>01/08/25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>24h</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00P0001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>C - (C 01/07/25_12H) - AM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>01/07/25</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 19:56)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,6 +645,56 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>03AN313</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BATERIA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>8334</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>SICOOB - (78KLM10 13/11/25_24/03/2020) - DF</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>24/03/2020</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>13/11/25</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática via Streamlit (13/11/2025 19:59)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +498,11 @@
           <t>STATUS</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>DATA_FIM_DT</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -526,7 +535,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>01/10/25</t>
+          <t>13/11/25</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -543,6 +552,9 @@
         <is>
           <t>DENTRO</t>
         </is>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>45931</v>
       </c>
     </row>
     <row r="3">
@@ -594,6 +606,9 @@
           <t>DENTRO</t>
         </is>
       </c>
+      <c r="M3" s="2" t="n">
+        <v>45870</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -644,6 +659,9 @@
           <t>DENTRO</t>
         </is>
       </c>
+      <c r="M4" s="2" t="n">
+        <v>45839</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -693,6 +711,9 @@
         <is>
           <t>DENTRO</t>
         </is>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>45974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:22)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,6 +716,57 @@
         <v>45974</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1234567</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>DS8K</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>SICOOB - (78KKT90 14/11/25_24/7) - DF</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>24/7</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:26)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -719,12 +719,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DF</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1234567</t>
+          <t>00P0098</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -732,27 +732,27 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>DS8K</t>
+          <t>A</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>SICOOB - (78KKT90 14/11/25_24/7) - DF</t>
+          <t>A - (A 01/11/25_12H) - GO</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>14/11/25</t>
+          <t>01/11/25</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>24/7</t>
+          <t>12H</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:30)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +767,57 @@
       </c>
       <c r="M6" t="inlineStr"/>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>00X0098</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>TESTEOLOBATO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>T - (T 01/11/25_12H) - DF</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:51)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -818,6 +818,57 @@
       </c>
       <c r="M7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TESTE00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>TESTE</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>T - (T 01/11/25_12H) - DF</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:54)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -821,12 +821,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DF</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TESTE00</t>
+          <t>TESTEGO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -834,7 +834,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>T</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -844,12 +844,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>T - (T 01/11/25_12H) - DF</t>
+          <t>T - (T 02/11/25_12H) - GO</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>01/11/25</t>
+          <t>02/11/25</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 19:56)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,6 +869,57 @@
       </c>
       <c r="M8" t="inlineStr"/>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TES1656</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>T - (T 03/11/25_24H) - DF</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>03/11/25</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>24H</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 20:00)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -877,7 +877,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TES1656</t>
+          <t>DIO1659</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -895,17 +895,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>T - (T 03/11/25_24H) - DF</t>
+          <t>T - (Y 12/11/25_12H) - DF</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>03/11/25</t>
+          <t>12/11/25</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>24H</t>
+          <t>12H</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 20:18)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,6 +920,57 @@
       </c>
       <c r="M9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DF00001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>TESTE1718</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>T - (T 03/11/25_12H) - DF</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>03/11/25</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (14/11/2025 20:41)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,6 +971,57 @@
       </c>
       <c r="M10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DF00002</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>X - (X 03/11/25_12H) - DF</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>03/11/25</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>14/11/25</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (15/11/2025 16:48)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="M2" s="2" t="n">
-        <v>45931</v>
+        <v>45974</v>
       </c>
     </row>
     <row r="3">
@@ -765,7 +765,9 @@
           <t>DENTRO</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" s="2" t="n">
+        <v>45962</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -816,17 +818,19 @@
           <t>DENTRO</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" s="2" t="n">
+        <v>45962</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>DF</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TESTEGO</t>
+          <t>DIO1659</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -844,12 +848,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>T - (T 02/11/25_12H) - GO</t>
+          <t>T - (Y 12/11/25_12H) - DF</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>02/11/25</t>
+          <t>12/11/25</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -867,7 +871,9 @@
           <t>DENTRO</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" s="2" t="n">
+        <v>45973</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -877,7 +883,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DIO1659</t>
+          <t>DF00001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -885,22 +891,22 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
+          <t>TESTE1718</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>T - (Y 12/11/25_12H) - DF</t>
+          <t>T - (T 03/11/25_12H) - DF</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>12/11/25</t>
+          <t>03/11/25</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -918,7 +924,9 @@
           <t>DENTRO</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" s="2" t="n">
+        <v>45964</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -928,7 +936,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DF00001</t>
+          <t>DF00002</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -936,17 +944,17 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>TESTE1718</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>T - (T 03/11/25_12H) - DF</t>
+          <t>X - (X 03/11/25_12H) - DF</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -969,58 +977,9 @@
           <t>DENTRO</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>DF</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>DF00002</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>X - (X 03/11/25_12H) - DF</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>03/11/25</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>12H</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>14/11/25</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>DENTRO</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M10" s="2" t="n">
+        <v>45964</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (15/11/2025 17:03)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,6 +981,57 @@
         <v>45964</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PA15110</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>HD 300 TB</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>44445</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>LIDER - (9809876 01/11/25_12H) - PA</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>15/11/25</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (17/11/2025 15:53)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1032,6 +1032,61 @@
       </c>
       <c r="M11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DF17110</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>125200</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>T - (T 30/11/26_24H) - DF</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>30/11/26</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>24H</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>17/11/25</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (18/11/2025 12:43)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1043,10 +1043,8 @@
           <t>DF17110</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>125200</t>
-        </is>
+      <c r="C12" t="n">
+        <v>125200</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -1086,6 +1084,61 @@
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DF18110</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0943000</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>T - (T 01/11/25_24H) - DF</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>24H</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>18/11/25</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Atualização automática SALDO_PECAS (19/11/2025 13:05)
</commit_message>
<xml_diff>
--- a/SALDO_PECAS.xlsx
+++ b/SALDO_PECAS.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,10 +1096,8 @@
           <t>DF18110</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0943000</t>
-        </is>
+      <c r="C13" t="n">
+        <v>943000</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
@@ -1139,6 +1137,61 @@
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DF19110</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1005000</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>X - (X 01/11/25_12H) - DF</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>12H</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>19/11/25</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>DENTRO</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>